<commit_message>
ETFI Project from Nqbao
</commit_message>
<xml_diff>
--- a/resources/input_mages/Demo/Data.xlsx
+++ b/resources/input_mages/Demo/Data.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NKKH\ThanhToanDotDau\Documents\Code-first\Bao\recognize-text-from-image-using-ocr\recognize-text-from-image-using-ocr\resources\input_mages\Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NKKH\ThanhToanDotDau\Documents\Code-first\Bao\recognize-text-from-image-using-ocr\ETFT\recognize-text-from-image-using-ocr\resources\input_mages\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5DCFC0-F382-4A7E-941B-4E4E2BC6C355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B576B8-2EF5-4249-A025-FF9DC90F6D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{75E87077-ED5E-47AD-B5E4-CE51FBFC320C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{75E87077-ED5E-47AD-B5E4-CE51FBFC320C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Tên:</t>
   </si>
@@ -112,6 +114,42 @@
   </si>
   <si>
     <t xml:space="preserve">Điểm TB </t>
+  </si>
+  <si>
+    <t>Nguyễn Thế Tài</t>
+  </si>
+  <si>
+    <t>THPT Lương Định Của</t>
+  </si>
+  <si>
+    <t>Có</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Tham gia</t>
+  </si>
+  <si>
+    <t>12A3</t>
+  </si>
+  <si>
+    <t>Học lực</t>
+  </si>
+  <si>
+    <t>Giỏi</t>
+  </si>
+  <si>
+    <t>Hoạt động</t>
+  </si>
+  <si>
+    <t>Cờ tướng</t>
+  </si>
+  <si>
+    <t>Điền kinh</t>
+  </si>
+  <si>
+    <t>Stt</t>
   </si>
 </sst>
 </file>
@@ -120,10 +158,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +190,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,7 +218,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -169,34 +226,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -515,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFB106B-0D36-4E75-9391-603922D35F65}">
   <dimension ref="D4:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,10 +658,10 @@
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -539,10 +669,10 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
@@ -557,11 +687,11 @@
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
@@ -581,7 +711,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="3">
@@ -591,15 +721,15 @@
         <v>6.7</v>
       </c>
       <c r="G9" s="3">
-        <f>(E9+F9)/2</f>
+        <f t="shared" ref="G9:G16" si="0">(E9+F9)/2</f>
         <v>7.75</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="3">
@@ -609,15 +739,15 @@
         <v>7.7</v>
       </c>
       <c r="G10" s="3">
-        <f>(E10+F10)/2</f>
+        <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="3">
@@ -627,15 +757,15 @@
         <v>7.8</v>
       </c>
       <c r="G11" s="3">
-        <f>(E11+F11)/2</f>
+        <f t="shared" si="0"/>
         <v>7.25</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="3">
@@ -645,15 +775,15 @@
         <v>8.9</v>
       </c>
       <c r="G12" s="3">
-        <f>(E12+F12)/2</f>
+        <f t="shared" si="0"/>
         <v>7.85</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="3">
@@ -663,15 +793,15 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="G13" s="3">
-        <f>(E13+F13)/2</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="3">
@@ -681,15 +811,15 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="G14" s="3">
-        <f>(E14+F14)/2</f>
+        <f t="shared" si="0"/>
         <v>9.3500000000000014</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="3">
@@ -699,15 +829,15 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="G15" s="3">
-        <f>(E15+F15)/2</f>
+        <f t="shared" si="0"/>
         <v>8.9499999999999993</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="4:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="3">
@@ -717,15 +847,15 @@
         <v>6.8</v>
       </c>
       <c r="G16" s="3">
-        <f>(E16+F16)/2</f>
+        <f t="shared" si="0"/>
         <v>7.85</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="4:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -743,15 +873,15 @@
       <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <f>AVERAGE(E9:E17)</f>
         <v>7.8124999999999991</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <f>AVERAGE(F9:F17)</f>
         <v>8.2750000000000004</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <f>(E18+F18)/2</f>
         <v>8.0437499999999993</v>
       </c>
@@ -767,4 +897,473 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84944C7F-89B8-4F17-8BB3-C413D37A17C0}">
+  <dimension ref="E3:P24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="50.21875" customWidth="1"/>
+    <col min="9" max="9" width="31.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="5:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E6" s="10"/>
+      <c r="F6" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="5:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E7" s="10"/>
+      <c r="F7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="5:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="5:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E9" s="10"/>
+      <c r="F9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="5:16" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="10"/>
+      <c r="F11" s="12">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="12">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="18"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E12" s="10"/>
+      <c r="F12" s="12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="12">
+        <v>7.8</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E13" s="10"/>
+      <c r="F13" s="12">
+        <v>3</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="12">
+        <v>6.7</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E14" s="10"/>
+      <c r="F14" s="12">
+        <v>4</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E15" s="10"/>
+      <c r="F15" s="12">
+        <v>5</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="12">
+        <v>5.4</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E16" s="10"/>
+      <c r="F16" s="12">
+        <v>6</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="12">
+        <v>8.9</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="18"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="10"/>
+      <c r="F17" s="12">
+        <v>7</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="12">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="18"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E18" s="10"/>
+      <c r="F18" s="12">
+        <v>8</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="12">
+        <v>8.9</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="18"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="5:16" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="E19" s="10"/>
+      <c r="F19" s="12">
+        <v>9</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="5:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E20" s="10"/>
+      <c r="F20" s="12">
+        <v>10</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="12">
+        <v>8.9</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="5:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E21" s="10"/>
+      <c r="F21" s="12">
+        <v>11</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+    </row>
+    <row r="23" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E803D8E2-E71A-4BEA-93D9-890E66CD0199}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>